<commit_message>
#3220 added 'Owner' and 'Owner Email' to data set
</commit_message>
<xml_diff>
--- a/seed/tests/data/building-performance-standards-sample-2023.xlsx
+++ b/seed/tests/data/building-performance-standards-sample-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achapin/seed/seed/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC5896B-5313-A54B-BA98-06C1911078C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1638AE-2EDF-5340-8D3D-EDDF1ECAB18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="3380" windowWidth="21600" windowHeight="20180" xr2:uid="{ABA70866-58E3-E741-9E6E-8CBE8BD4F008}"/>
+    <workbookView xWindow="2900" yWindow="2820" windowWidth="38400" windowHeight="20180" xr2:uid="{ABA70866-58E3-E741-9E6E-8CBE8BD4F008}"/>
   </bookViews>
   <sheets>
     <sheet name="BPS Data" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t>Property Name</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Medical Office</t>
   </si>
   <si>
-    <t>Building ID</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total GHG Emissions Intensity </t>
   </si>
   <si>
@@ -155,13 +152,103 @@
   </si>
   <si>
     <t>Audit Template Building ID</t>
+  </si>
+  <si>
+    <t>Portfolio Manager Building ID</t>
+  </si>
+  <si>
+    <t>21537666</t>
+  </si>
+  <si>
+    <t>21537667</t>
+  </si>
+  <si>
+    <t>21537668</t>
+  </si>
+  <si>
+    <t>21537669</t>
+  </si>
+  <si>
+    <t>21537670</t>
+  </si>
+  <si>
+    <t>21537671</t>
+  </si>
+  <si>
+    <t>21537672</t>
+  </si>
+  <si>
+    <t>21537673</t>
+  </si>
+  <si>
+    <t>21537674</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Owner Email</t>
+  </si>
+  <si>
+    <t>Company A</t>
+  </si>
+  <si>
+    <t>Company B</t>
+  </si>
+  <si>
+    <t>Company C</t>
+  </si>
+  <si>
+    <t>Company D</t>
+  </si>
+  <si>
+    <t>Company E</t>
+  </si>
+  <si>
+    <t>Company F</t>
+  </si>
+  <si>
+    <t>Company G</t>
+  </si>
+  <si>
+    <t>Company H</t>
+  </si>
+  <si>
+    <t>Company I</t>
+  </si>
+  <si>
+    <t>admin@companya.com</t>
+  </si>
+  <si>
+    <t>admin@companyb.com</t>
+  </si>
+  <si>
+    <t>admin@companyc.com</t>
+  </si>
+  <si>
+    <t>admin@companyd.com</t>
+  </si>
+  <si>
+    <t>admin@companye.com</t>
+  </si>
+  <si>
+    <t>admin@companyf.com</t>
+  </si>
+  <si>
+    <t>admin@companyg.com</t>
+  </si>
+  <si>
+    <t>admin@companyh.com</t>
+  </si>
+  <si>
+    <t>admin@companyi.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -201,6 +288,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -234,12 +329,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -249,8 +345,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{4367F287-F053-B14B-BB78-7F2A1A8270CC}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{FC32E4A8-5101-754C-BA01-BA4BA25B0A66}"/>
@@ -643,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AAF8DA-FAFC-5247-8BBA-26096DB3751B}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,12 +753,12 @@
     <col min="4" max="4" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -669,582 +767,653 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>19</v>
+      <c r="I1" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>11911</v>
       </c>
-      <c r="B2" s="2">
-        <v>70339502439620</v>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
         <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
       </c>
       <c r="H2">
         <v>10027</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2">
         <v>193850</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>19</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>129</v>
       </c>
-      <c r="L2" s="4">
+      <c r="N2" s="4">
         <v>44635</v>
       </c>
-      <c r="M2" s="4">
+      <c r="O2" s="4">
         <v>44926</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>20</v>
       </c>
-      <c r="O2">
-        <v>2027</v>
-      </c>
-      <c r="P2">
+      <c r="Q2">
+        <v>2027</v>
+      </c>
+      <c r="R2">
         <v>120</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>2027</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>12227</v>
       </c>
-      <c r="B3">
-        <v>70339508188740</v>
+      <c r="B3" t="s">
+        <v>41</v>
       </c>
       <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
       </c>
       <c r="H3">
         <v>91342</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3">
         <v>30000</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>12</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>70</v>
       </c>
-      <c r="L3" s="4">
+      <c r="N3" s="4">
         <v>44594</v>
       </c>
-      <c r="M3" s="4">
+      <c r="O3" s="4">
         <v>44926</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>10</v>
       </c>
-      <c r="O3">
-        <v>2027</v>
-      </c>
-      <c r="P3">
+      <c r="Q3">
+        <v>2027</v>
+      </c>
+      <c r="R3">
         <v>56</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>2027</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>17971</v>
       </c>
-      <c r="B4">
-        <v>70339467993140</v>
+      <c r="B4" t="s">
+        <v>42</v>
       </c>
       <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H4">
         <v>10468</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4">
         <v>79000</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>50</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>63</v>
       </c>
-      <c r="L4" s="4">
+      <c r="N4" s="4">
         <v>44594</v>
       </c>
-      <c r="M4" s="4">
+      <c r="O4" s="4">
         <v>44926</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>40</v>
       </c>
-      <c r="O4">
-        <v>2027</v>
-      </c>
-      <c r="P4">
+      <c r="Q4">
+        <v>2027</v>
+      </c>
+      <c r="R4">
         <v>45</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>2027</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>21381</v>
       </c>
-      <c r="B5">
-        <v>70339516372420</v>
+      <c r="B5" t="s">
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
         <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
       </c>
       <c r="H5">
         <v>10006</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5">
         <v>368315</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>55</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>87.2</v>
       </c>
-      <c r="L5" s="4">
+      <c r="N5" s="4">
         <v>44631</v>
       </c>
-      <c r="M5" s="4">
+      <c r="O5" s="4">
         <v>44926</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>45</v>
       </c>
-      <c r="O5">
-        <v>2027</v>
-      </c>
-      <c r="P5">
+      <c r="Q5">
+        <v>2027</v>
+      </c>
+      <c r="R5">
         <v>70</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>2027</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>21404</v>
       </c>
-      <c r="B6">
-        <v>70339452621140</v>
+      <c r="B6" t="s">
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6">
         <v>10459</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6">
         <v>51190</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>44</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>106.3</v>
       </c>
-      <c r="L6" s="4">
+      <c r="N6" s="4">
         <v>44562</v>
       </c>
-      <c r="M6" s="4">
+      <c r="O6" s="4">
         <v>44926</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>37</v>
       </c>
-      <c r="O6">
-        <v>2027</v>
-      </c>
-      <c r="P6">
+      <c r="Q6">
+        <v>2027</v>
+      </c>
+      <c r="R6">
         <v>85</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>2027</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>21405</v>
       </c>
-      <c r="B7">
-        <v>70339516221660</v>
+      <c r="B7" t="s">
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
         <v>17</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
       </c>
       <c r="H7">
         <v>10006</v>
       </c>
-      <c r="I7">
+      <c r="I7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K7">
         <v>447442</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>66</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>56.4</v>
       </c>
-      <c r="L7" s="4">
+      <c r="N7" s="4">
         <v>44622</v>
       </c>
-      <c r="M7" s="4">
+      <c r="O7" s="4">
         <v>44926</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>50</v>
       </c>
-      <c r="O7">
-        <v>2027</v>
-      </c>
-      <c r="P7">
+      <c r="Q7">
+        <v>2027</v>
+      </c>
+      <c r="R7">
         <v>45</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>2027</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>21368</v>
       </c>
-      <c r="B8">
-        <v>70339463823000</v>
+      <c r="B8" t="s">
+        <v>46</v>
       </c>
       <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8">
         <v>94107</v>
       </c>
-      <c r="I8">
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8">
         <v>8352</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>30</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>270</v>
       </c>
-      <c r="L8" s="4">
+      <c r="N8" s="4">
         <v>44623</v>
       </c>
-      <c r="M8" s="4">
+      <c r="O8" s="4">
         <v>44926</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>25</v>
       </c>
-      <c r="O8">
-        <v>2027</v>
-      </c>
-      <c r="P8">
+      <c r="Q8">
+        <v>2027</v>
+      </c>
+      <c r="R8">
         <v>200</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>2027</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>21378</v>
       </c>
-      <c r="B9">
-        <v>70339513510300</v>
+      <c r="B9" t="s">
+        <v>47</v>
       </c>
       <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9">
         <v>94133</v>
       </c>
-      <c r="I9">
+      <c r="I9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9">
         <v>40017</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>54</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>77.7</v>
       </c>
-      <c r="L9" s="4">
+      <c r="N9" s="4">
         <v>44624</v>
       </c>
-      <c r="M9" s="4">
+      <c r="O9" s="4">
         <v>44926</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>45</v>
       </c>
-      <c r="O9">
-        <v>2027</v>
-      </c>
-      <c r="P9">
+      <c r="Q9">
+        <v>2027</v>
+      </c>
+      <c r="R9">
         <v>60</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>2027</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>21426</v>
       </c>
-      <c r="B10">
-        <v>70339508400460</v>
+      <c r="B10" t="s">
+        <v>48</v>
       </c>
       <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10">
         <v>94124</v>
       </c>
-      <c r="I10">
+      <c r="I10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K10">
         <v>53000</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>49</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>58.1</v>
       </c>
-      <c r="L10" s="4">
+      <c r="N10" s="4">
         <v>44625</v>
       </c>
-      <c r="M10" s="4">
+      <c r="O10" s="4">
         <v>44926</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>40</v>
       </c>
-      <c r="O10">
-        <v>2027</v>
-      </c>
-      <c r="P10">
+      <c r="Q10">
+        <v>2027</v>
+      </c>
+      <c r="R10">
         <v>45</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>2027</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="I2:K10">
+  <conditionalFormatting sqref="K2:M10">
     <cfRule type="expression" dxfId="10" priority="31" stopIfTrue="1">
-      <formula>$P2="Yes"</formula>
+      <formula>$R2="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="K2:K10">
     <cfRule type="cellIs" dxfId="9" priority="30" operator="notBetween">
       <formula>1000</formula>
       <formula>1000000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:K10">
+  <conditionalFormatting sqref="K2:M10">
     <cfRule type="expression" dxfId="8" priority="28" stopIfTrue="1">
-      <formula>$N2="Yes"</formula>
+      <formula>$P2="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K10">
+  <conditionalFormatting sqref="M2:M10">
     <cfRule type="cellIs" dxfId="7" priority="29" operator="notBetween">
       <formula>40</formula>
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:O6 O2:Q10">
+  <conditionalFormatting sqref="P2:Q6 Q2:S10">
     <cfRule type="expression" dxfId="6" priority="21" stopIfTrue="1">
-      <formula>$R2="Yes"</formula>
+      <formula>$T2="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:O6 O2:Q10">
+  <conditionalFormatting sqref="P2:Q6 Q2:S10">
     <cfRule type="expression" dxfId="5" priority="19" stopIfTrue="1">
-      <formula>$Q2="Yes"</formula>
+      <formula>$S2="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P10">
+  <conditionalFormatting sqref="R2:R10">
     <cfRule type="cellIs" dxfId="4" priority="20" operator="notBetween">
       <formula>40</formula>
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N7:O8 N9:N10">
+  <conditionalFormatting sqref="P7:Q8 P9:P10">
     <cfRule type="expression" dxfId="3" priority="22" stopIfTrue="1">
-      <formula>$R6="Yes"</formula>
+      <formula>$T6="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N7:O8 N9:N10">
+  <conditionalFormatting sqref="P7:Q8 P9:P10">
     <cfRule type="expression" dxfId="2" priority="23" stopIfTrue="1">
-      <formula>$Q6="Yes"</formula>
+      <formula>$S6="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O9:O10">
+  <conditionalFormatting sqref="Q9:Q10">
     <cfRule type="expression" dxfId="1" priority="13" stopIfTrue="1">
-      <formula>$R8="Yes"</formula>
+      <formula>$T8="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O9:O10">
+  <conditionalFormatting sqref="Q9:Q10">
     <cfRule type="expression" dxfId="0" priority="14" stopIfTrue="1">
-      <formula>$Q8="Yes"</formula>
+      <formula>$S8="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{29AFF97E-6AB5-EC44-BE73-1B011B77495F}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{966F41B2-9567-FF42-8E84-E6A3533EB236}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{0CBB3623-D677-884B-B1C4-65CA25FA0599}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{FC691147-C2FE-BB49-BFFA-8FD7D35B36E1}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{F6144DAC-AAC3-3F4E-BA5E-3D3F9CE41765}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{5C5C2F30-2FF7-9947-8D32-6B90330617A4}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{DB846E0E-DC17-7B4D-9422-DE787F4C0D75}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{7300CF6A-C66E-1D4C-8ADD-CCF8F8B5D475}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{FB11B44F-CFDC-7C40-BD55-B0DB50DEABEA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#3220 updated BPS sample data targets
</commit_message>
<xml_diff>
--- a/seed/tests/data/building-performance-standards-sample-2023.xlsx
+++ b/seed/tests/data/building-performance-standards-sample-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achapin/seed/seed/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1638AE-2EDF-5340-8D3D-EDDF1ECAB18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32103423-4F92-0D4F-85AA-2B48CDA32B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="2820" windowWidth="38400" windowHeight="20180" xr2:uid="{ABA70866-58E3-E741-9E6E-8CBE8BD4F008}"/>
+    <workbookView xWindow="7300" yWindow="6760" windowWidth="38400" windowHeight="20180" xr2:uid="{ABA70866-58E3-E741-9E6E-8CBE8BD4F008}"/>
   </bookViews>
   <sheets>
     <sheet name="BPS Data" sheetId="2" r:id="rId1"/>
@@ -744,7 +744,7 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="P1" sqref="P1:S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,13 +859,13 @@
         <v>44926</v>
       </c>
       <c r="P2">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="Q2">
         <v>2027</v>
       </c>
       <c r="R2">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="S2">
         <v>2027</v>
@@ -918,7 +918,7 @@
         <v>44926</v>
       </c>
       <c r="P3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="Q3">
         <v>2027</v>
@@ -977,13 +977,13 @@
         <v>44926</v>
       </c>
       <c r="P4">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="Q4">
         <v>2027</v>
       </c>
       <c r="R4">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="S4">
         <v>2027</v>
@@ -1036,13 +1036,13 @@
         <v>44926</v>
       </c>
       <c r="P5">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="Q5">
         <v>2027</v>
       </c>
       <c r="R5">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="S5">
         <v>2027</v>
@@ -1095,13 +1095,13 @@
         <v>44926</v>
       </c>
       <c r="P6">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="Q6">
         <v>2027</v>
       </c>
       <c r="R6">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="S6">
         <v>2027</v>
@@ -1154,13 +1154,13 @@
         <v>44926</v>
       </c>
       <c r="P7">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="Q7">
         <v>2027</v>
       </c>
       <c r="R7">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="S7">
         <v>2027</v>
@@ -1213,13 +1213,13 @@
         <v>44926</v>
       </c>
       <c r="P8">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="Q8">
         <v>2027</v>
       </c>
       <c r="R8">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="S8">
         <v>2027</v>
@@ -1272,7 +1272,7 @@
         <v>44926</v>
       </c>
       <c r="P9">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="Q9">
         <v>2027</v>
@@ -1331,13 +1331,13 @@
         <v>44926</v>
       </c>
       <c r="P10">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Q10">
         <v>2027</v>
       </c>
       <c r="R10">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S10">
         <v>2027</v>

</xml_diff>